<commit_message>
update firmware 3.13 y php 8.1
</commit_message>
<xml_diff>
--- a/app/files/mimasoft_files/client_1/project_1/form_8/LAG_EC5Exportaciónaérea_plantilla.xlsx
+++ b/app/files/mimasoft_files/client_1/project_1/form_8/LAG_EC5Exportaciónaérea_plantilla.xlsx
@@ -907,49 +907,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" t="s">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
     </row>
@@ -957,46 +957,46 @@
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="0">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="0" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="0">
         <v>2023</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="0" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="0" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1051,174 +1051,174 @@
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1">
+      <c r="A1" s="0">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="0">
         <v>2023</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2">
+      <c r="A2" s="0">
         <v>2</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="0">
         <v>2024</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="0" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3">
+      <c r="A3" s="0">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4">
+      <c r="A4" s="0">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5">
+      <c r="A5" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6">
+      <c r="A6" s="0">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7">
+      <c r="A7" s="0">
         <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8">
+      <c r="A8" s="0">
         <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9">
+      <c r="A9" s="0">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10">
+      <c r="A10" s="0">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11">
+      <c r="A11" s="0">
         <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12">
+      <c r="A12" s="0">
         <v>157</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13">
+      <c r="A13" s="0">
         <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14">
+      <c r="A14" s="0">
         <v>172</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15">
+      <c r="A15" s="0">
         <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16">
+      <c r="A16" s="0">
         <v>176</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17">
+      <c r="A17" s="0">
         <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18">
+      <c r="A18" s="0">
         <v>235</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19">
+      <c r="A19" s="0">
         <v>272</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20">
+      <c r="A20" s="0">
         <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21">
+      <c r="A21" s="0">
         <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22">
+      <c r="A22" s="0">
         <v>416</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23">
+      <c r="A23" s="0">
         <v>501</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24">
+      <c r="A24" s="0">
         <v>724</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25">
+      <c r="A25" s="0">
         <v>729</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26">
+      <c r="A26" s="0">
         <v>810</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27">
+      <c r="A27" s="0">
         <v>865</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28">
+      <c r="A28" s="0">
         <v>992</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29">
+      <c r="A29" s="0">
         <v>996</v>
       </c>
     </row>

</xml_diff>